<commit_message>
ran fim after small change to medicare formula
</commit_message>
<xml_diff>
--- a/results/04-2023/comparison-deflators-04-2023.xlsx
+++ b/results/04-2023/comparison-deflators-04-2023.xlsx
@@ -897,13 +897,13 @@
         <v>0.0054</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.0105</v>
+        <v>-0.0335</v>
       </c>
       <c r="R7" t="n">
-        <v>0.0215</v>
+        <v>-0.0665</v>
       </c>
       <c r="S7" t="n">
-        <v>-5.4038</v>
+        <v>-5.4026</v>
       </c>
     </row>
     <row r="8">
@@ -1428,13 +1428,13 @@
         <v>0.0354</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.1756</v>
+        <v>0.1316</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.0445</v>
+        <v>-0.1326</v>
       </c>
       <c r="S16" t="n">
-        <v>-72.6398</v>
+        <v>-72.6385</v>
       </c>
     </row>
     <row r="17">
@@ -2549,13 +2549,13 @@
         <v>-0.0212</v>
       </c>
       <c r="Q35" t="n">
-        <v>-0.0203</v>
+        <v>-0.0643</v>
       </c>
       <c r="R35" t="n">
-        <v>-0.0195</v>
+        <v>-0.1075</v>
       </c>
       <c r="S35" t="n">
-        <v>-0.0006</v>
+        <v>0.0007</v>
       </c>
     </row>
     <row r="36">
@@ -3080,13 +3080,13 @@
         <v>0.1485</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.147</v>
+        <v>0.103</v>
       </c>
       <c r="R44" t="n">
-        <v>-0.051</v>
+        <v>-0.139</v>
       </c>
       <c r="S44" t="n">
-        <v>-0.4966</v>
+        <v>-0.4953</v>
       </c>
     </row>
     <row r="45">

</xml_diff>

<commit_message>
ran fim after speaking to louise
adjusted according to mpi and brought down other judgmental line items
</commit_message>
<xml_diff>
--- a/results/04-2023/comparison-deflators-04-2023.xlsx
+++ b/results/04-2023/comparison-deflators-04-2023.xlsx
@@ -761,31 +761,31 @@
         <v>0.2406</v>
       </c>
       <c r="K5" t="n">
-        <v>0.7965</v>
+        <v>-0.3802</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.0543</v>
+        <v>-0.1156</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.0468</v>
+        <v>-0.0439</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.2968</v>
+        <v>-0.2949</v>
       </c>
       <c r="O5" t="n">
-        <v>-0.4273</v>
+        <v>-0.4257</v>
       </c>
       <c r="P5" t="n">
-        <v>-0.0633</v>
+        <v>-0.0613</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.0522</v>
+        <v>-0.0515</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.3905</v>
+        <v>-0.3876</v>
       </c>
       <c r="S5" t="n">
-        <v>-34.1547</v>
+        <v>-32.9216</v>
       </c>
     </row>
     <row r="6">
@@ -879,31 +879,31 @@
         <v>-0.0208</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0183</v>
+        <v>0.0179</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0037</v>
+        <v>0.0029</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.0019</v>
+        <v>-0.0022</v>
       </c>
       <c r="N7" t="n">
         <v>-0.0845</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.0121</v>
+        <v>-0.0113</v>
       </c>
       <c r="P7" t="n">
-        <v>0.0054</v>
+        <v>0.007</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.0335</v>
+        <v>-0.0111</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.0665</v>
+        <v>-0.0244</v>
       </c>
       <c r="S7" t="n">
-        <v>-5.4026</v>
+        <v>-5.4036</v>
       </c>
     </row>
     <row r="8">
@@ -938,31 +938,31 @@
         <v>0.1494</v>
       </c>
       <c r="K8" t="n">
-        <v>0.2862</v>
+        <v>0.3134</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1881</v>
+        <v>0.2152</v>
       </c>
       <c r="M8" t="n">
-        <v>0.2507</v>
+        <v>0.2641</v>
       </c>
       <c r="N8" t="n">
-        <v>0.5235</v>
+        <v>0.5368</v>
       </c>
       <c r="O8" t="n">
-        <v>0.5152</v>
+        <v>0.5283</v>
       </c>
       <c r="P8" t="n">
-        <v>0.5439</v>
+        <v>0.5569</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.4964</v>
+        <v>0.5092</v>
       </c>
       <c r="R8" t="n">
-        <v>0.2581</v>
+        <v>0.2708</v>
       </c>
       <c r="S8" t="n">
-        <v>7.6778</v>
+        <v>7.6505</v>
       </c>
     </row>
     <row r="9">
@@ -1174,31 +1174,31 @@
         <v>0.1206</v>
       </c>
       <c r="K12" t="n">
-        <v>0.3406</v>
+        <v>0.225</v>
       </c>
       <c r="L12" t="n">
-        <v>0.3823</v>
+        <v>0.2688</v>
       </c>
       <c r="M12" t="n">
-        <v>0.0976</v>
+        <v>-0.0137</v>
       </c>
       <c r="N12" t="n">
-        <v>0.0086</v>
+        <v>-0.1003</v>
       </c>
       <c r="O12" t="n">
-        <v>-0.0902</v>
+        <v>-0.0852</v>
       </c>
       <c r="P12" t="n">
-        <v>-0.0749</v>
+        <v>-0.0702</v>
       </c>
       <c r="Q12" t="n">
-        <v>-0.0395</v>
+        <v>-0.0351</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.0772</v>
+        <v>-0.0729</v>
       </c>
       <c r="S12" t="n">
-        <v>-6.8028</v>
+        <v>-6.6924</v>
       </c>
     </row>
     <row r="13">
@@ -1410,31 +1410,31 @@
         <v>-0.2404</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.8901</v>
+        <v>-1.2456</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.0217</v>
+        <v>-0.1857</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.0588</v>
+        <v>-0.1632</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.2646</v>
+        <v>-0.3603</v>
       </c>
       <c r="O16" t="n">
-        <v>0.0008</v>
+        <v>0.0317</v>
       </c>
       <c r="P16" t="n">
-        <v>0.0354</v>
+        <v>0.0696</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.1316</v>
+        <v>0.1879</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.1326</v>
+        <v>-0.0504</v>
       </c>
       <c r="S16" t="n">
-        <v>-72.6385</v>
+        <v>-72.2455</v>
       </c>
     </row>
     <row r="17">
@@ -1528,31 +1528,31 @@
         <v>-0.139</v>
       </c>
       <c r="K18" t="n">
-        <v>0.8155</v>
+        <v>-0.1144</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.1213</v>
+        <v>-0.1186</v>
       </c>
       <c r="M18" t="n">
-        <v>-0.071</v>
+        <v>-0.0684</v>
       </c>
       <c r="N18" t="n">
-        <v>-0.2617</v>
+        <v>-0.2598</v>
       </c>
       <c r="O18" t="n">
-        <v>-0.3737</v>
+        <v>-0.3725</v>
       </c>
       <c r="P18" t="n">
-        <v>-0.0142</v>
+        <v>-0.0132</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.0124</v>
+        <v>0.0133</v>
       </c>
       <c r="R18" t="n">
-        <v>-0.3171</v>
+        <v>-0.3159</v>
       </c>
       <c r="S18" t="n">
-        <v>-7.7689</v>
+        <v>-6.8434</v>
       </c>
     </row>
     <row r="19">
@@ -1764,31 +1764,31 @@
         <v>0.2551</v>
       </c>
       <c r="K22" t="n">
-        <v>-0.8619</v>
+        <v>0.0681</v>
       </c>
       <c r="L22" t="n">
-        <v>0.1258</v>
+        <v>0.123</v>
       </c>
       <c r="M22" t="n">
-        <v>-0.0077</v>
+        <v>-0.0103</v>
       </c>
       <c r="N22" t="n">
-        <v>0.202</v>
+        <v>0.2002</v>
       </c>
       <c r="O22" t="n">
-        <v>0.2928</v>
+        <v>0.2917</v>
       </c>
       <c r="P22" t="n">
-        <v>-0.0689</v>
+        <v>-0.0699</v>
       </c>
       <c r="Q22" t="n">
-        <v>-0.0989</v>
+        <v>-0.0998</v>
       </c>
       <c r="R22" t="n">
-        <v>0.2283</v>
+        <v>0.2271</v>
       </c>
       <c r="S22" t="n">
-        <v>-36.5076</v>
+        <v>-37.433</v>
       </c>
     </row>
     <row r="23">
@@ -1882,31 +1882,31 @@
         <v>0.0083</v>
       </c>
       <c r="K24" t="n">
-        <v>0.015</v>
+        <v>0.0149</v>
       </c>
       <c r="L24" t="n">
-        <v>0.1235</v>
+        <v>0.1232</v>
       </c>
       <c r="M24" t="n">
-        <v>0.0767</v>
+        <v>0.0766</v>
       </c>
       <c r="N24" t="n">
         <v>0.0873</v>
       </c>
       <c r="O24" t="n">
-        <v>-0.0185</v>
+        <v>-0.0182</v>
       </c>
       <c r="P24" t="n">
-        <v>-0.0678</v>
+        <v>-0.0672</v>
       </c>
       <c r="Q24" t="n">
-        <v>-0.0544</v>
+        <v>-0.0456</v>
       </c>
       <c r="R24" t="n">
-        <v>-0.0526</v>
+        <v>-0.036</v>
       </c>
       <c r="S24" t="n">
-        <v>-0.7102</v>
+        <v>-0.7106</v>
       </c>
     </row>
     <row r="25">
@@ -2177,31 +2177,31 @@
         <v>-0.0268</v>
       </c>
       <c r="K29" t="n">
-        <v>0.0066</v>
+        <v>-0.0131</v>
       </c>
       <c r="L29" t="n">
-        <v>0.0185</v>
+        <v>0.006</v>
       </c>
       <c r="M29" t="n">
-        <v>0.027</v>
+        <v>0.0207</v>
       </c>
       <c r="N29" t="n">
-        <v>0.0221</v>
+        <v>0.0219</v>
       </c>
       <c r="O29" t="n">
-        <v>0.013</v>
+        <v>0.0242</v>
       </c>
       <c r="P29" t="n">
-        <v>0.0052</v>
+        <v>0.0184</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.0006</v>
+        <v>0.0086</v>
       </c>
       <c r="R29" t="n">
-        <v>-0.0026</v>
+        <v>0.0021</v>
       </c>
       <c r="S29" t="n">
-        <v>-0.0921</v>
+        <v>-0.0885</v>
       </c>
     </row>
     <row r="30">
@@ -2413,31 +2413,31 @@
         <v>0.7084</v>
       </c>
       <c r="K33" t="n">
-        <v>0.8467</v>
+        <v>-0.33</v>
       </c>
       <c r="L33" t="n">
-        <v>-0.0018</v>
+        <v>-0.0631</v>
       </c>
       <c r="M33" t="n">
-        <v>-0.0024</v>
+        <v>0.0005</v>
       </c>
       <c r="N33" t="n">
-        <v>-0.0007</v>
+        <v>0.0012</v>
       </c>
       <c r="O33" t="n">
-        <v>0.0007</v>
+        <v>0.0022</v>
       </c>
       <c r="P33" t="n">
-        <v>-0.0015</v>
+        <v>0.0005</v>
       </c>
       <c r="Q33" t="n">
-        <v>-0.0018</v>
+        <v>-0.0011</v>
       </c>
       <c r="R33" t="n">
-        <v>0</v>
+        <v>0.0029</v>
       </c>
       <c r="S33" t="n">
-        <v>-1.304</v>
+        <v>-0.0709</v>
       </c>
     </row>
     <row r="34">
@@ -2531,31 +2531,31 @@
         <v>0.0576</v>
       </c>
       <c r="K35" t="n">
-        <v>0.0167</v>
+        <v>0.0163</v>
       </c>
       <c r="L35" t="n">
-        <v>0.0457</v>
+        <v>0.0449</v>
       </c>
       <c r="M35" t="n">
-        <v>0.0395</v>
+        <v>0.0392</v>
       </c>
       <c r="N35" t="n">
-        <v>-0.0217</v>
+        <v>-0.0216</v>
       </c>
       <c r="O35" t="n">
-        <v>0.0119</v>
+        <v>0.0127</v>
       </c>
       <c r="P35" t="n">
-        <v>-0.0212</v>
+        <v>-0.0197</v>
       </c>
       <c r="Q35" t="n">
-        <v>-0.0643</v>
+        <v>-0.042</v>
       </c>
       <c r="R35" t="n">
-        <v>-0.1075</v>
+        <v>-0.0654</v>
       </c>
       <c r="S35" t="n">
-        <v>0.0007</v>
+        <v>-0.0003</v>
       </c>
     </row>
     <row r="36">
@@ -2590,31 +2590,31 @@
         <v>0.2942</v>
       </c>
       <c r="K36" t="n">
-        <v>0.2784</v>
+        <v>0.3056</v>
       </c>
       <c r="L36" t="n">
-        <v>0.1256</v>
+        <v>0.1527</v>
       </c>
       <c r="M36" t="n">
-        <v>0.1255</v>
+        <v>0.139</v>
       </c>
       <c r="N36" t="n">
-        <v>0.1212</v>
+        <v>0.1345</v>
       </c>
       <c r="O36" t="n">
-        <v>0.118</v>
+        <v>0.1312</v>
       </c>
       <c r="P36" t="n">
-        <v>0.1145</v>
+        <v>0.1275</v>
       </c>
       <c r="Q36" t="n">
-        <v>0.1141</v>
+        <v>0.127</v>
       </c>
       <c r="R36" t="n">
-        <v>-0.0213</v>
+        <v>-0.0085</v>
       </c>
       <c r="S36" t="n">
-        <v>-0.3111</v>
+        <v>-0.3384</v>
       </c>
     </row>
     <row r="37">
@@ -2826,31 +2826,31 @@
         <v>0.1027</v>
       </c>
       <c r="K40" t="n">
-        <v>0.2148</v>
+        <v>0.0992</v>
       </c>
       <c r="L40" t="n">
-        <v>0.2104</v>
+        <v>0.0969</v>
       </c>
       <c r="M40" t="n">
-        <v>0.2079</v>
+        <v>0.0967</v>
       </c>
       <c r="N40" t="n">
-        <v>0.1043</v>
+        <v>-0.0046</v>
       </c>
       <c r="O40" t="n">
-        <v>-0.0094</v>
+        <v>-0.0044</v>
       </c>
       <c r="P40" t="n">
-        <v>-0.0088</v>
+        <v>-0.0042</v>
       </c>
       <c r="Q40" t="n">
-        <v>-0.0086</v>
+        <v>-0.0042</v>
       </c>
       <c r="R40" t="n">
-        <v>-0.008</v>
+        <v>-0.0037</v>
       </c>
       <c r="S40" t="n">
-        <v>-0.1712</v>
+        <v>-0.0608</v>
       </c>
     </row>
     <row r="41">
@@ -3062,31 +3062,31 @@
         <v>1.219</v>
       </c>
       <c r="K44" t="n">
-        <v>0.6706</v>
+        <v>0.3152</v>
       </c>
       <c r="L44" t="n">
-        <v>0.4358</v>
+        <v>0.2717</v>
       </c>
       <c r="M44" t="n">
-        <v>0.4236</v>
+        <v>0.3192</v>
       </c>
       <c r="N44" t="n">
-        <v>0.2777</v>
+        <v>0.182</v>
       </c>
       <c r="O44" t="n">
-        <v>0.1547</v>
+        <v>0.1856</v>
       </c>
       <c r="P44" t="n">
-        <v>0.1485</v>
+        <v>0.1827</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.103</v>
+        <v>0.1593</v>
       </c>
       <c r="R44" t="n">
-        <v>-0.139</v>
+        <v>-0.0568</v>
       </c>
       <c r="S44" t="n">
-        <v>-0.4953</v>
+        <v>-0.1023</v>
       </c>
     </row>
     <row r="45">
@@ -3180,31 +3180,31 @@
         <v>0.3164</v>
       </c>
       <c r="K46" t="n">
-        <v>0.8469</v>
+        <v>-0.083</v>
       </c>
       <c r="L46" t="n">
-        <v>-0.0024</v>
+        <v>0.0003</v>
       </c>
       <c r="M46" t="n">
-        <v>-0.0026</v>
+        <v>0</v>
       </c>
       <c r="N46" t="n">
-        <v>-0.0004</v>
+        <v>0.0014</v>
       </c>
       <c r="O46" t="n">
-        <v>0.0012</v>
+        <v>0.0023</v>
       </c>
       <c r="P46" t="n">
-        <v>-0.001</v>
+        <v>-0.0001</v>
       </c>
       <c r="Q46" t="n">
-        <v>-0.0012</v>
+        <v>-0.0003</v>
       </c>
       <c r="R46" t="n">
-        <v>0.0007</v>
+        <v>0.0019</v>
       </c>
       <c r="S46" t="n">
-        <v>-1.0514</v>
+        <v>-0.1259</v>
       </c>
     </row>
     <row r="47">
@@ -3416,31 +3416,31 @@
         <v>-0.0687</v>
       </c>
       <c r="K50" t="n">
-        <v>-0.8465</v>
+        <v>0.0834</v>
       </c>
       <c r="L50" t="n">
-        <v>0.0024</v>
+        <v>-0.0003</v>
       </c>
       <c r="M50" t="n">
-        <v>0.0033</v>
+        <v>0.0007</v>
       </c>
       <c r="N50" t="n">
-        <v>0.0009</v>
+        <v>-0.0009</v>
       </c>
       <c r="O50" t="n">
-        <v>-0.0005</v>
+        <v>-0.0017</v>
       </c>
       <c r="P50" t="n">
-        <v>0.0017</v>
+        <v>0.0008</v>
       </c>
       <c r="Q50" t="n">
-        <v>0.0019</v>
+        <v>0.001</v>
       </c>
       <c r="R50" t="n">
-        <v>0</v>
+        <v>-0.0012</v>
       </c>
       <c r="S50" t="n">
-        <v>1.4204</v>
+        <v>0.4949</v>
       </c>
     </row>
     <row r="51">
@@ -3534,31 +3534,31 @@
         <v>-0.0248</v>
       </c>
       <c r="K52" t="n">
-        <v>0.0095</v>
+        <v>0.0093</v>
       </c>
       <c r="L52" t="n">
-        <v>-0.0264</v>
+        <v>-0.0267</v>
       </c>
       <c r="M52" t="n">
-        <v>-0.027</v>
+        <v>-0.0272</v>
       </c>
       <c r="N52" t="n">
         <v>-0.0038</v>
       </c>
       <c r="O52" t="n">
-        <v>-0.0372</v>
+        <v>-0.0369</v>
       </c>
       <c r="P52" t="n">
-        <v>-0.0038</v>
+        <v>-0.0032</v>
       </c>
       <c r="Q52" t="n">
-        <v>-0.0036</v>
+        <v>0.0052</v>
       </c>
       <c r="R52" t="n">
-        <v>-0.0035</v>
+        <v>0.0132</v>
       </c>
       <c r="S52" t="n">
-        <v>0.0328</v>
+        <v>0.0324</v>
       </c>
     </row>
     <row r="53">
@@ -3829,31 +3829,31 @@
         <v>0.0008</v>
       </c>
       <c r="K57" t="n">
-        <v>0.0128</v>
+        <v>-0.0069</v>
       </c>
       <c r="L57" t="n">
-        <v>0.0114</v>
+        <v>-0.001</v>
       </c>
       <c r="M57" t="n">
-        <v>0.011</v>
+        <v>0.0047</v>
       </c>
       <c r="N57" t="n">
-        <v>0.0098</v>
+        <v>0.0096</v>
       </c>
       <c r="O57" t="n">
-        <v>0.0055</v>
+        <v>0.0167</v>
       </c>
       <c r="P57" t="n">
-        <v>0.0027</v>
+        <v>0.0159</v>
       </c>
       <c r="Q57" t="n">
-        <v>0.0022</v>
+        <v>0.0102</v>
       </c>
       <c r="R57" t="n">
-        <v>0.0013</v>
+        <v>0.0061</v>
       </c>
       <c r="S57" t="n">
-        <v>-0.0126</v>
+        <v>-0.009</v>
       </c>
     </row>
     <row r="58">

</xml_diff>